<commit_message>
updated backlog, added beginning of start and end screen
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\norton402\Documents\Cita 331 project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3E2C1B-206D-49DB-86E2-920294438DC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF5D9F8-865C-4624-B9BC-65BDD2955689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{946D40EF-4548-4C07-9DC7-C31E8865D345}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Use Cases</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>Hours per day</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -97,12 +106,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -127,6 +148,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9AC437-7C81-4C75-B4BD-D7C7F51DF92A}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -575,7 +598,9 @@
     <col min="1" max="1" width="30.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="16" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="16" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
@@ -741,6 +766,9 @@
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -751,6 +779,9 @@
       </c>
       <c r="C8" s="1">
         <v>1</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
@@ -763,6 +794,9 @@
       <c r="C9" s="1">
         <v>1</v>
       </c>
+      <c r="D9" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -774,6 +808,9 @@
       <c r="C10" s="1">
         <v>1</v>
       </c>
+      <c r="D10" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -784,6 +821,9 @@
       </c>
       <c r="C11" s="1">
         <v>1</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionality to the start and end screen
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\norton402\Documents\Cita 331 project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF5D9F8-865C-4624-B9BC-65BDD2955689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2502C9E3-4FAA-4EC4-A6B3-80FF4C4F98A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{946D40EF-4548-4C07-9DC7-C31E8865D345}"/>
   </bookViews>
@@ -165,6 +165,1133 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 1'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Optimal Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 1'!$B$1:$O$1</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>44079</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44080</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44081</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44082</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44083</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44084</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44085</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44086</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44087</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44088</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44089</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44090</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44091</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44092</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1'!$B$2:$O$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.076923076923077</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.153846153846153</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.2307692307692299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.3076923076923066</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.3846153846153832</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.4615384615384599</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5384615384615365</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.6153846153846132</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.6923076923076898</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.7692307692307665</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.8461538461538434</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.92307692307692024</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2.886579864025407E-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D4FA-4F40-BE88-CDBCDFD88742}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 1'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 1'!$B$1:$O$1</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>44079</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44080</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44081</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44082</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44083</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44084</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44085</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44086</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44087</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44088</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44089</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44090</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44091</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44092</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1'!$B$3:$O$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D4FA-4F40-BE88-CDBCDFD88742}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="153432336"/>
+        <c:axId val="88849840"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="153432336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="88849840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="88849840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="153432336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>136524</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>330199</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>69849</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24B7DDF7-EDC9-472D-B00D-D3DE243D22DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -589,8 +1716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9AC437-7C81-4C75-B4BD-D7C7F51DF92A}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -651,7 +1778,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3">
         <v>12</v>
@@ -712,7 +1839,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3">
         <v>12</v>
@@ -744,8 +1871,15 @@
       <c r="K3" s="4">
         <v>9</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
+      <c r="L3" s="4">
+        <v>9</v>
+      </c>
+      <c r="M3" s="4">
+        <v>7</v>
+      </c>
+      <c r="N3" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -808,8 +1942,8 @@
       <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>16</v>
+      <c r="D10" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
@@ -822,11 +1956,12 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>16</v>
+      <c r="D11" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working store buttons to navigate to and from game Restructured files
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\norton402\Documents\Cita 331 project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2502C9E3-4FAA-4EC4-A6B3-80FF4C4F98A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9945C938-6A94-48F3-9A0E-139652D71E2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{946D40EF-4548-4C07-9DC7-C31E8865D345}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Use Cases</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Hours per day</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -106,18 +103,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -138,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -149,7 +140,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,6 +487,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1717,7 +1710,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1880,6 +1873,9 @@
       <c r="N3" s="4">
         <v>3</v>
       </c>
+      <c r="O3" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -1901,7 +1897,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
@@ -1914,8 +1910,8 @@
       <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>18</v>
+      <c r="D8" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
@@ -1929,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
@@ -1942,8 +1938,8 @@
       <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>18</v>
+      <c r="D10" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
@@ -1956,8 +1952,8 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>18</v>
+      <c r="D11" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All regions are clickable buttons
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\norton402\Documents\Cita 331 project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A23FBC-BB54-4912-8801-6F8130D0986A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1679AC-4D4E-4425-89BE-486E2074689A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{946D40EF-4548-4C07-9DC7-C31E8865D345}"/>
   </bookViews>
@@ -35,15 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Use Cases</t>
   </si>
   <si>
     <t>Time Estimate</t>
-  </si>
-  <si>
-    <t>Sprint Assigned</t>
   </si>
   <si>
     <t>See map broken up by DEC regions</t>
@@ -94,9 +91,6 @@
     <t>Insects spread at a reasonable rate</t>
   </si>
   <si>
-    <t>Create counters on game screen to show infection</t>
-  </si>
-  <si>
     <t>Regions change color based on infection</t>
   </si>
   <si>
@@ -104,6 +98,9 @@
   </si>
   <si>
     <t>In progress</t>
+  </si>
+  <si>
+    <t>Each region is clickable to show infection and statistics</t>
   </si>
 </sst>
 </file>
@@ -151,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -164,6 +161,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1608,10 +1606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D27D7C-B2EE-4D3E-859D-D7B7524B6EE3}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1628,13 +1626,10 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -1642,7 +1637,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -1650,7 +1645,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -1658,7 +1653,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1666,7 +1661,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1674,11 +1669,20 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1751,7 +1755,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3">
         <v>12</v>
@@ -1812,7 +1816,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>12</v>
@@ -1859,7 +1863,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <f>12/13</f>
@@ -1874,51 +1878,51 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1">
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1">
         <v>3</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1929,15 +1933,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721CEA7C-7589-4D9A-BD78-7615EEDE1AD4}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="15" width="9.453125" bestFit="1" customWidth="1"/>
@@ -1989,67 +1993,67 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="7">
         <f>B2-$B$5</f>
-        <v>10.153846153846153</v>
+        <v>11.076923076923077</v>
       </c>
       <c r="D2" s="7">
         <f t="shared" ref="D2:O2" si="0">C2-$B$5</f>
-        <v>9.3076923076923066</v>
+        <v>10.153846153846153</v>
       </c>
       <c r="E2" s="7">
         <f t="shared" si="0"/>
-        <v>8.4615384615384599</v>
+        <v>9.2307692307692299</v>
       </c>
       <c r="F2" s="7">
         <f t="shared" si="0"/>
-        <v>7.6153846153846141</v>
+        <v>8.3076923076923066</v>
       </c>
       <c r="G2" s="7">
         <f t="shared" si="0"/>
-        <v>6.7692307692307683</v>
+        <v>7.3846153846153832</v>
       </c>
       <c r="H2" s="7">
         <f t="shared" si="0"/>
-        <v>5.9230769230769225</v>
+        <v>6.4615384615384599</v>
       </c>
       <c r="I2" s="7">
         <f t="shared" si="0"/>
-        <v>5.0769230769230766</v>
+        <v>5.5384615384615365</v>
       </c>
       <c r="J2" s="7">
         <f t="shared" si="0"/>
-        <v>4.2307692307692308</v>
+        <v>4.6153846153846132</v>
       </c>
       <c r="K2" s="7">
         <f t="shared" si="0"/>
-        <v>3.3846153846153846</v>
+        <v>3.6923076923076898</v>
       </c>
       <c r="L2" s="7">
         <f t="shared" si="0"/>
-        <v>2.5384615384615383</v>
+        <v>2.7692307692307665</v>
       </c>
       <c r="M2" s="7">
         <f t="shared" si="0"/>
-        <v>1.6923076923076921</v>
+        <v>1.8461538461538434</v>
       </c>
       <c r="N2" s="7">
         <f t="shared" si="0"/>
-        <v>0.84615384615384592</v>
+        <v>0.92307692307692024</v>
       </c>
       <c r="O2" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2.886579864025407E-15</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>11</v>
@@ -2063,14 +2067,23 @@
       <c r="E3">
         <v>11</v>
       </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5">
-        <f xml:space="preserve"> 11/13</f>
-        <v>0.84615384615384615</v>
+        <f xml:space="preserve"> 12/13</f>
+        <v>0.92307692307692313</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
@@ -2078,43 +2091,32 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
         <v>20</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started on getting infection information to show when region is clicked Updated backlog
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\norton402\Documents\Cita 331 project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1679AC-4D4E-4425-89BE-486E2074689A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F89CD9-3A46-4357-A7D7-66CA63D8C4D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{946D40EF-4548-4C07-9DC7-C31E8865D345}"/>
   </bookViews>
@@ -1606,10 +1606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D27D7C-B2EE-4D3E-859D-D7B7524B6EE3}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1683,6 +1683,12 @@
         <v>4</v>
       </c>
       <c r="C8" s="8"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <f xml:space="preserve"> SUM(B2:B8)</f>
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1935,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721CEA7C-7589-4D9A-BD78-7615EEDE1AD4}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2076,6 +2082,12 @@
       <c r="H3">
         <v>8</v>
       </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
Clicking regions shows healthy trees, infected trees, and percent infected
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\norton402\Documents\Cita 331 project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F89CD9-3A46-4357-A7D7-66CA63D8C4D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3350244B-1D89-49AA-9322-FE288252F57C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{946D40EF-4548-4C07-9DC7-C31E8865D345}"/>
   </bookViews>
@@ -1942,7 +1942,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2088,6 +2088,12 @@
       <c r="J3">
         <v>6</v>
       </c>
+      <c r="K3">
+        <v>6</v>
+      </c>
+      <c r="L3">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -2127,8 +2133,8 @@
       <c r="B10">
         <v>8</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>20</v>
+      <c r="C10" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
infection spreads within the regions
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\norton402\Documents\Cita 331 project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3350244B-1D89-49AA-9322-FE288252F57C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CA0DA3-23A4-4E6A-B57F-B0C4686C11D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{946D40EF-4548-4C07-9DC7-C31E8865D345}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{946D40EF-4548-4C07-9DC7-C31E8865D345}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Use Cases</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Each region is clickable to show infection and statistics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insects spread between regions </t>
   </si>
 </sst>
 </file>
@@ -1606,10 +1609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D27D7C-B2EE-4D3E-859D-D7B7524B6EE3}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1684,10 +1687,18 @@
       </c>
       <c r="C8" s="8"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B10">
-        <f xml:space="preserve"> SUM(B2:B8)</f>
-        <v>33</v>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <f xml:space="preserve"> SUM(B2:B9)</f>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1941,8 +1952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721CEA7C-7589-4D9A-BD78-7615EEDE1AD4}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2094,6 +2105,12 @@
       <c r="L3">
         <v>4</v>
       </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
updated product backlog for current sprint and prepared to start on the sprint
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\norton402\Documents\Cita 331 project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CA0DA3-23A4-4E6A-B57F-B0C4686C11D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060032DC-E3E5-4C2F-A52A-F3582848A6AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{946D40EF-4548-4C07-9DC7-C31E8865D345}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{946D40EF-4548-4C07-9DC7-C31E8865D345}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint 3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Use Cases</t>
   </si>
@@ -97,13 +98,16 @@
     <t>Estimate</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>Each region is clickable to show infection and statistics</t>
   </si>
   <si>
     <t xml:space="preserve">Insects spread between regions </t>
+  </si>
+  <si>
+    <t>Resize start screen for web gl</t>
+  </si>
+  <si>
+    <t>Progress</t>
   </si>
 </sst>
 </file>
@@ -119,7 +123,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,12 +133,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -162,9 +160,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,7 +724,653 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 2 Burndown</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Optimal Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 2'!$B$1:$O$1</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>44093</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44094</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44095</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44097</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44098</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44099</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44101</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44102</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44103</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44104</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44106</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$B$2:$O$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.076923076923077</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.153846153846153</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.2307692307692299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.3076923076923066</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.3846153846153832</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.4615384615384599</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5384615384615365</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.6153846153846132</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.6923076923076898</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.7692307692307665</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.8461538461538434</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.92307692307692024</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2.886579864025407E-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1B36-49A6-9B2B-155A7896EB6B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 2'!$B$1:$O$1</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>44093</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44094</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44095</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44097</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44098</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44099</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44101</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44102</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44103</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44104</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44106</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$B$3:$O$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1B36-49A6-9B2B-155A7896EB6B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1723727488"/>
+        <c:axId val="1710113984"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="1723727488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1710113984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1710113984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Hours</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1723727488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1271,6 +1913,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1292,6 +2450,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24B7DDF7-EDC9-472D-B00D-D3DE243D22DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>282574</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>647699</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>165099</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3834B61B-B69A-4277-8353-87A4316CB0FC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1609,10 +2808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D27D7C-B2EE-4D3E-859D-D7B7524B6EE3}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1622,7 +2821,7 @@
     <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1630,7 +2829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1638,67 +2837,50 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B11">
-        <f xml:space="preserve"> SUM(B2:B9)</f>
-        <v>35</v>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <f xml:space="preserve"> SUM(B2:B8)</f>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1711,7 +2893,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1952,8 +3134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721CEA7C-7589-4D9A-BD78-7615EEDE1AD4}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2015,55 +3197,55 @@
       <c r="B2">
         <v>12</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <f>B2-$B$5</f>
         <v>11.076923076923077</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <f t="shared" ref="D2:O2" si="0">C2-$B$5</f>
         <v>10.153846153846153</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <f t="shared" si="0"/>
         <v>9.2307692307692299</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <f t="shared" si="0"/>
         <v>8.3076923076923066</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <f t="shared" si="0"/>
         <v>7.3846153846153832</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="6">
         <f t="shared" si="0"/>
         <v>6.4615384615384599</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="6">
         <f t="shared" si="0"/>
         <v>5.5384615384615365</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="6">
         <f t="shared" si="0"/>
         <v>4.6153846153846132</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="6">
         <f t="shared" si="0"/>
         <v>3.6923076923076898</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="6">
         <f t="shared" si="0"/>
         <v>2.7692307692307665</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="6">
         <f t="shared" si="0"/>
         <v>1.8461538461538434</v>
       </c>
-      <c r="N2" s="7">
+      <c r="N2" s="6">
         <f t="shared" si="0"/>
         <v>0.92307692307692024</v>
       </c>
-      <c r="O2" s="7">
+      <c r="O2" s="6">
         <f t="shared" si="0"/>
         <v>-2.886579864025407E-15</v>
       </c>
@@ -2073,13 +3255,13 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>11</v>
@@ -2110,6 +3292,9 @@
       </c>
       <c r="N3">
         <v>1</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
@@ -2139,19 +3324,217 @@
       <c r="B9">
         <v>4</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>20</v>
+      <c r="C9" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2E014E-C511-424A-861C-D78082ACB806}">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="34.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2">
+        <v>44107</v>
+      </c>
+      <c r="C1" s="2">
+        <v>44108</v>
+      </c>
+      <c r="D1" s="2">
+        <v>44109</v>
+      </c>
+      <c r="E1" s="2">
+        <v>44110</v>
+      </c>
+      <c r="F1" s="2">
+        <v>44111</v>
+      </c>
+      <c r="G1" s="2">
+        <v>44112</v>
+      </c>
+      <c r="H1" s="2">
+        <v>44113</v>
+      </c>
+      <c r="I1" s="2">
+        <v>44114</v>
+      </c>
+      <c r="J1" s="2">
+        <v>44115</v>
+      </c>
+      <c r="K1" s="2">
+        <v>44116</v>
+      </c>
+      <c r="L1" s="2">
+        <v>44117</v>
+      </c>
+      <c r="M1" s="2">
+        <v>44118</v>
+      </c>
+      <c r="N1" s="2">
+        <v>44119</v>
+      </c>
+      <c r="O1" s="2">
+        <v>44120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1">
+        <v>11</v>
+      </c>
+      <c r="C2" s="6">
+        <f>B2-$B$5</f>
+        <v>10.153846153846153</v>
+      </c>
+      <c r="D2" s="6">
+        <f t="shared" ref="D2:O2" si="0">C2-$B$5</f>
+        <v>9.3076923076923066</v>
+      </c>
+      <c r="E2" s="6">
+        <f t="shared" si="0"/>
+        <v>8.4615384615384599</v>
+      </c>
+      <c r="F2" s="6">
+        <f t="shared" si="0"/>
+        <v>7.6153846153846141</v>
+      </c>
+      <c r="G2" s="6">
+        <f t="shared" si="0"/>
+        <v>6.7692307692307683</v>
+      </c>
+      <c r="H2" s="6">
+        <f t="shared" si="0"/>
+        <v>5.9230769230769225</v>
+      </c>
+      <c r="I2" s="6">
+        <f t="shared" si="0"/>
+        <v>5.0769230769230766</v>
+      </c>
+      <c r="J2" s="6">
+        <f t="shared" si="0"/>
+        <v>4.2307692307692308</v>
+      </c>
+      <c r="K2" s="6">
+        <f t="shared" si="0"/>
+        <v>3.3846153846153846</v>
+      </c>
+      <c r="L2" s="6">
+        <f t="shared" si="0"/>
+        <v>2.5384615384615383</v>
+      </c>
+      <c r="M2" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6923076923076921</v>
+      </c>
+      <c r="N2" s="6">
+        <f t="shared" si="0"/>
+        <v>0.84615384615384592</v>
+      </c>
+      <c r="O2" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <f xml:space="preserve"> 11 / 13</f>
+        <v>0.84615384615384615</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on getting money as game goes on
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\norton402\Documents\Cita 331 project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF579FA-48FB-43A0-85B0-DA3498C1F5B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0590DF6D-6BED-4674-AEFB-75B53AC4BC4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{946D40EF-4548-4C07-9DC7-C31E8865D345}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{946D40EF-4548-4C07-9DC7-C31E8865D345}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sprint 2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sprint 3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint 4" sheetId="5" r:id="rId2"/>
+    <sheet name="Sprint 1" sheetId="2" r:id="rId3"/>
+    <sheet name="Sprint 2" sheetId="3" r:id="rId4"/>
+    <sheet name="Sprint 3" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>Use Cases</t>
   </si>
@@ -109,6 +110,27 @@
   <si>
     <t>Progress</t>
   </si>
+  <si>
+    <t>Create options menu</t>
+  </si>
+  <si>
+    <t>Create news lines</t>
+  </si>
+  <si>
+    <t>Estimates</t>
+  </si>
+  <si>
+    <t>Hours Per Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual Trend </t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain money as you play </t>
+  </si>
 </sst>
 </file>
 
@@ -123,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +155,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -161,6 +189,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -179,6 +208,552 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint 4 Burndown</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 4'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Optimal Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 4'!$B$1:$O$1</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>44121</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44122</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44123</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44124</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44126</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44127</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44129</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44130</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44131</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44132</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44133</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44134</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 4'!$B$2:$O$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.923076923076923</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.846153846153847</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.76923076923077</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.6923076923076934</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6153846153846168</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.5384615384615401</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.4615384615384635</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.3846153846153868</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.3076923076923102</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.2307692307692335</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1538461538461569</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.07692307692308</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AA84-4E78-8730-4651E3C830C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 4'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Trend </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 4'!$B$1:$O$1</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>44121</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44122</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44123</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44124</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44126</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44127</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44129</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44130</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44131</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44132</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44133</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44134</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 4'!$B$3:$O$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AA84-4E78-8730-4651E3C830C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1949160351"/>
+        <c:axId val="1863573759"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="1949160351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1863573759"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1863573759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1949160351"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -724,7 +1299,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1330,7 +1905,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2001,8 +2576,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2110,6 +2725,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -2120,6 +2740,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -2151,6 +2776,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2505,7 +3133,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2613,11 +3241,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -2628,11 +3251,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -2664,9 +3282,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3536,7 +4151,564 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>301625</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>492125</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>22225</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5880555B-5412-4C0C-8D35-C06E25E36BCE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3577,7 +4749,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3618,7 +4790,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3959,7 +5131,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4001,20 +5173,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-    </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -4028,7 +5200,7 @@
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10">
         <f xml:space="preserve"> SUM(B2:B8)</f>
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -4037,11 +5209,234 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91FD6068-3BE7-4603-BA44-D41628E5D2D7}">
+  <dimension ref="A1:O10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="15" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B1" s="2">
+        <v>44121</v>
+      </c>
+      <c r="C1" s="2">
+        <v>44122</v>
+      </c>
+      <c r="D1" s="2">
+        <v>44123</v>
+      </c>
+      <c r="E1" s="2">
+        <v>44124</v>
+      </c>
+      <c r="F1" s="2">
+        <v>44125</v>
+      </c>
+      <c r="G1" s="2">
+        <v>44126</v>
+      </c>
+      <c r="H1" s="2">
+        <v>44127</v>
+      </c>
+      <c r="I1" s="2">
+        <v>44128</v>
+      </c>
+      <c r="J1" s="2">
+        <v>44129</v>
+      </c>
+      <c r="K1" s="2">
+        <v>44130</v>
+      </c>
+      <c r="L1" s="2">
+        <v>44131</v>
+      </c>
+      <c r="M1" s="2">
+        <v>44132</v>
+      </c>
+      <c r="N1" s="2">
+        <v>44133</v>
+      </c>
+      <c r="O1" s="2">
+        <v>44134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6">
+        <f>B2 - $B$5</f>
+        <v>12.923076923076923</v>
+      </c>
+      <c r="D2" s="6">
+        <f>C2 - $B$5</f>
+        <v>11.846153846153847</v>
+      </c>
+      <c r="E2" s="6">
+        <f t="shared" ref="E2:N2" si="0">D2 - $B$5</f>
+        <v>10.76923076923077</v>
+      </c>
+      <c r="F2" s="6">
+        <f t="shared" si="0"/>
+        <v>9.6923076923076934</v>
+      </c>
+      <c r="G2" s="6">
+        <f t="shared" si="0"/>
+        <v>8.6153846153846168</v>
+      </c>
+      <c r="H2" s="6">
+        <f t="shared" si="0"/>
+        <v>7.5384615384615401</v>
+      </c>
+      <c r="I2" s="6">
+        <f t="shared" si="0"/>
+        <v>6.4615384615384635</v>
+      </c>
+      <c r="J2" s="6">
+        <f t="shared" si="0"/>
+        <v>5.3846153846153868</v>
+      </c>
+      <c r="K2" s="6">
+        <f t="shared" si="0"/>
+        <v>4.3076923076923102</v>
+      </c>
+      <c r="L2" s="6">
+        <f t="shared" si="0"/>
+        <v>3.2307692307692335</v>
+      </c>
+      <c r="M2" s="6">
+        <f t="shared" si="0"/>
+        <v>2.1538461538461569</v>
+      </c>
+      <c r="N2" s="6">
+        <f t="shared" si="0"/>
+        <v>1.07692307692308</v>
+      </c>
+      <c r="O2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1">
+        <v>14</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>9</v>
+      </c>
+      <c r="M3">
+        <v>9</v>
+      </c>
+      <c r="N3">
+        <v>8</v>
+      </c>
+      <c r="O3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <f>14/13</f>
+        <v>1.0769230769230769</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9AC437-7C81-4C75-B4BD-D7C7F51DF92A}">
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4278,7 +5673,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721CEA7C-7589-4D9A-BD78-7615EEDE1AD4}">
   <dimension ref="A1:O10"/>
   <sheetViews>
@@ -4493,11 +5888,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2E014E-C511-424A-861C-D78082ACB806}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
game saves between scenes
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\norton402\Documents\Cita 331 project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C01F4E1-1C7B-4E77-8C5E-280289B68DE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA18224-2DF5-4D7D-AB37-2CA85E5A1341}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{946D40EF-4548-4C07-9DC7-C31E8865D345}"/>
   </bookViews>
@@ -144,7 +144,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -200,7 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -219,6 +219,549 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint 5 Burndown</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 5'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Optimal Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 5'!$B$1:$O$1</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>44135</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44137</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44138</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44139</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44140</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44141</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44142</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44143</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44144</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44145</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44146</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44147</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44148</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 5'!$B$2:$O$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.923076923076923</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.846153846153847</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.76923076923077</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.6923076923076934</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6153846153846168</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.5384615384615401</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.4615384615384635</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.3846153846153868</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.3076923076923102</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.2307692307692335</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1538461538461569</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.07692307692308</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.1086244689504383E-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4CCB-419E-AD03-D76BC6AD10BF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 5'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Trend </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 5'!$B$1:$O$1</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>44135</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44137</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44138</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44139</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44140</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44141</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44142</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44143</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44144</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44145</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44146</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44147</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44148</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 5'!$B$3:$O$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4CCB-419E-AD03-D76BC6AD10BF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="275530176"/>
+        <c:axId val="453669296"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="275530176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="453669296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="453669296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="275530176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -764,7 +1307,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1310,7 +1853,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1916,7 +2459,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2627,6 +3170,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3144,7 +3727,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3252,6 +3835,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -3262,6 +3850,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -3293,6 +3886,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3647,7 +4243,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3755,11 +4351,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -3770,11 +4361,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -3806,9 +4392,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4678,7 +5261,564 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>434975</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF67F419-A9AA-48C2-A5AB-E3E54CCFAAA4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4719,7 +5859,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4760,7 +5900,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4801,7 +5941,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5215,8 +6355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C987EAD7-BA63-4D61-9132-22CFCDB53293}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5336,6 +6476,45 @@
       <c r="A3" t="s">
         <v>28</v>
       </c>
+      <c r="B3">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>12</v>
+      </c>
+      <c r="G3">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>11</v>
+      </c>
+      <c r="I3">
+        <v>11</v>
+      </c>
+      <c r="J3">
+        <v>11</v>
+      </c>
+      <c r="K3">
+        <v>11</v>
+      </c>
+      <c r="L3">
+        <v>8</v>
+      </c>
+      <c r="M3">
+        <v>8</v>
+      </c>
+      <c r="N3">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -5381,6 +6560,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Final changes to last sprint backlog
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\norton402\Documents\Cita 331 project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA18224-2DF5-4D7D-AB37-2CA85E5A1341}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A6434E-D0F3-44AA-BA14-5EFFD36CF174}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{946D40EF-4548-4C07-9DC7-C31E8865D345}"/>
   </bookViews>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">Hours per day </t>
   </si>
   <si>
-    <t>In Progress</t>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -155,7 +155,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,12 +165,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -187,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -199,7 +193,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -549,6 +542,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5782,15 +5778,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>98425</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>434975</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>165099</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6355,8 +6351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C987EAD7-BA63-4D61-9132-22CFCDB53293}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6419,55 +6415,55 @@
       <c r="B2">
         <v>14</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <f>B2-$B$5</f>
         <v>12.923076923076923</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <f>C2-$B$5</f>
         <v>11.846153846153847</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <f t="shared" ref="E2:N2" si="0">D2-$B$5</f>
         <v>10.76923076923077</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <f t="shared" si="0"/>
         <v>9.6923076923076934</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <f t="shared" si="0"/>
         <v>8.6153846153846168</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7">
         <f t="shared" si="0"/>
         <v>7.5384615384615401</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="7">
         <f t="shared" si="0"/>
         <v>6.4615384615384635</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="7">
         <f t="shared" si="0"/>
         <v>5.3846153846153868</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="7">
         <f t="shared" si="0"/>
         <v>4.3076923076923102</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="7">
         <f t="shared" si="0"/>
         <v>3.2307692307692335</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M2" s="7">
         <f t="shared" si="0"/>
         <v>2.1538461538461569</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="7">
         <f t="shared" si="0"/>
         <v>1.07692307692308</v>
       </c>
-      <c r="O2" s="8">
+      <c r="O2" s="7">
         <f>N2-$B$5</f>
         <v>3.1086244689504383E-15</v>
       </c>
@@ -6515,12 +6511,15 @@
       <c r="N3">
         <v>4</v>
       </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <f>14/13</f>
         <v>1.0769230769230769</v>
       </c>
@@ -6543,7 +6542,7 @@
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6554,7 +6553,7 @@
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Able to continue or start new game, also round infection percent
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\norton402\Documents\Cita 331 project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A6434E-D0F3-44AA-BA14-5EFFD36CF174}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97F8F80-AFB9-4083-AF5C-5D223BD1FB0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{946D40EF-4548-4C07-9DC7-C31E8865D345}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Sprint 5" sheetId="6" r:id="rId2"/>
-    <sheet name="Sprint 4" sheetId="5" r:id="rId3"/>
-    <sheet name="Sprint 1" sheetId="2" r:id="rId4"/>
-    <sheet name="Sprint 2" sheetId="3" r:id="rId5"/>
-    <sheet name="Sprint 3" sheetId="4" r:id="rId6"/>
+    <sheet name="Sprint 6" sheetId="7" r:id="rId2"/>
+    <sheet name="Sprint 5" sheetId="6" r:id="rId3"/>
+    <sheet name="Sprint 4" sheetId="5" r:id="rId4"/>
+    <sheet name="Sprint 1" sheetId="2" r:id="rId5"/>
+    <sheet name="Sprint 2" sheetId="3" r:id="rId6"/>
+    <sheet name="Sprint 3" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
   <si>
     <t>Use Cases</t>
   </si>
@@ -58,16 +59,7 @@
     <t>Create difficulty options</t>
   </si>
   <si>
-    <t>Create color blind settings in options</t>
-  </si>
-  <si>
-    <t>Create volume settings in options</t>
-  </si>
-  <si>
     <t>Have realistic options in the store to slow the spread</t>
-  </si>
-  <si>
-    <t>Create a tutorial</t>
   </si>
   <si>
     <t>Create a start screen</t>
@@ -138,6 +130,9 @@
   <si>
     <t>DONE</t>
   </si>
+  <si>
+    <t>In Progress</t>
+  </si>
 </sst>
 </file>
 
@@ -155,7 +150,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +160,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -181,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -194,6 +195,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6275,10 +6277,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D27D7C-B2EE-4D3E-859D-D7B7524B6EE3}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6296,50 +6298,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B10">
-        <f xml:space="preserve"> SUM(B3:B8)</f>
-        <v>21</v>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <f xml:space="preserve"> SUM('Sprint 6'!B8:B9)</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -6348,11 +6310,226 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6DE7ECD-A4B6-43A6-97C1-6F7018720662}">
+  <dimension ref="A1:P9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="9.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B1" s="2">
+        <v>44156</v>
+      </c>
+      <c r="C1" s="2">
+        <v>44157</v>
+      </c>
+      <c r="D1" s="2">
+        <v>44158</v>
+      </c>
+      <c r="E1" s="2">
+        <v>44159</v>
+      </c>
+      <c r="F1" s="2">
+        <v>44160</v>
+      </c>
+      <c r="G1" s="2">
+        <v>44161</v>
+      </c>
+      <c r="H1" s="2">
+        <v>44162</v>
+      </c>
+      <c r="I1" s="2">
+        <v>44163</v>
+      </c>
+      <c r="J1" s="2">
+        <v>44164</v>
+      </c>
+      <c r="K1" s="2">
+        <v>44165</v>
+      </c>
+      <c r="L1" s="2">
+        <v>44166</v>
+      </c>
+      <c r="M1" s="2">
+        <v>44167</v>
+      </c>
+      <c r="N1" s="2">
+        <v>44168</v>
+      </c>
+      <c r="O1" s="2">
+        <v>44169</v>
+      </c>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6">
+        <f>B2 - $B$5</f>
+        <v>7.384615384615385</v>
+      </c>
+      <c r="D2" s="6">
+        <f t="shared" ref="D2:P2" si="0">C2 - $B$5</f>
+        <v>6.7692307692307701</v>
+      </c>
+      <c r="E2" s="6">
+        <f t="shared" si="0"/>
+        <v>6.1538461538461551</v>
+      </c>
+      <c r="F2" s="6">
+        <f t="shared" si="0"/>
+        <v>5.5384615384615401</v>
+      </c>
+      <c r="G2" s="6">
+        <f t="shared" si="0"/>
+        <v>4.9230769230769251</v>
+      </c>
+      <c r="H2" s="6">
+        <f t="shared" si="0"/>
+        <v>4.3076923076923102</v>
+      </c>
+      <c r="I2" s="6">
+        <f t="shared" si="0"/>
+        <v>3.6923076923076947</v>
+      </c>
+      <c r="J2" s="6">
+        <f t="shared" si="0"/>
+        <v>3.0769230769230793</v>
+      </c>
+      <c r="K2" s="6">
+        <f t="shared" si="0"/>
+        <v>2.4615384615384639</v>
+      </c>
+      <c r="L2" s="6">
+        <f t="shared" si="0"/>
+        <v>1.8461538461538485</v>
+      </c>
+      <c r="M2" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2307692307692331</v>
+      </c>
+      <c r="N2" s="6">
+        <f t="shared" si="0"/>
+        <v>0.61538461538461764</v>
+      </c>
+      <c r="O2" s="6">
+        <f t="shared" si="0"/>
+        <v>2.2204460492503131E-15</v>
+      </c>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <v>6</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>5</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="6">
+        <f xml:space="preserve"> 8/13</f>
+        <v>0.61538461538461542</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C987EAD7-BA63-4D61-9132-22CFCDB53293}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6410,7 +6587,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>14</v>
@@ -6470,7 +6647,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>14</v>
@@ -6517,7 +6694,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" s="7">
         <f>14/13</f>
@@ -6529,10 +6706,10 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
@@ -6543,18 +6720,18 @@
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -6563,7 +6740,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91FD6068-3BE7-4603-BA44-D41628E5D2D7}">
   <dimension ref="A1:O10"/>
   <sheetViews>
@@ -6623,7 +6800,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>14</v>
@@ -6682,7 +6859,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>14</v>
@@ -6729,7 +6906,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <f>14/13</f>
@@ -6741,43 +6918,43 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>5</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -6786,7 +6963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9AC437-7C81-4C75-B4BD-D7C7F51DF92A}">
   <dimension ref="A1:P11"/>
   <sheetViews>
@@ -6852,7 +7029,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3">
         <v>12</v>
@@ -6913,7 +7090,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>12</v>
@@ -6960,7 +7137,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <f>12/13</f>
@@ -6975,7 +7152,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
@@ -6986,7 +7163,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
@@ -6997,29 +7174,29 @@
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1">
         <v>3</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -7028,7 +7205,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721CEA7C-7589-4D9A-BD78-7615EEDE1AD4}">
   <dimension ref="A1:O10"/>
   <sheetViews>
@@ -7090,7 +7267,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -7150,7 +7327,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>12</v>
@@ -7197,7 +7374,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <f xml:space="preserve"> 12/13</f>
@@ -7209,32 +7386,32 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -7243,7 +7420,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2E014E-C511-424A-861C-D78082ACB806}">
   <dimension ref="A1:O11"/>
   <sheetViews>
@@ -7305,7 +7482,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1">
         <v>11</v>
@@ -7365,7 +7542,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <v>11</v>
@@ -7421,32 +7598,32 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
@@ -7457,7 +7634,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>